<commit_message>
update museumstation videocue list
</commit_message>
<xml_diff>
--- a/analysis/museumstation/all_cdm_items.xlsx
+++ b/analysis/museumstation/all_cdm_items.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brialong/Documents/GitHub/kiddraw/analysis/museumstation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2413F97B-FD88-6B4E-9EFA-2E003F10E83B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CB31BF-ED3F-6349-8153-AA2E15205439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{09828A9D-5624-9A45-82AB-F087D8BCCF48}"/>
+    <workbookView xWindow="3320" yWindow="3320" windowWidth="28040" windowHeight="17040" xr2:uid="{09828A9D-5624-9A45-82AB-F087D8BCCF48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$39</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="66">
   <si>
     <t>a bear</t>
   </si>
@@ -162,33 +162,6 @@
     <t>cdm_run_v3_or_v4</t>
   </si>
   <si>
-    <t>vehicle</t>
-  </si>
-  <si>
-    <t>big animal</t>
-  </si>
-  <si>
-    <t>small animal</t>
-  </si>
-  <si>
-    <t>small object</t>
-  </si>
-  <si>
-    <t>furniture</t>
-  </si>
-  <si>
-    <t>place</t>
-  </si>
-  <si>
-    <t>person</t>
-  </si>
-  <si>
-    <t>plant</t>
-  </si>
-  <si>
-    <t>small oanimal</t>
-  </si>
-  <si>
     <t>item</t>
   </si>
   <si>
@@ -204,9 +177,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>maybe</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -228,10 +198,40 @@
     <t>a bed</t>
   </si>
   <si>
-    <t>a television</t>
-  </si>
-  <si>
     <t>alt quickname name</t>
+  </si>
+  <si>
+    <t>a bee</t>
+  </si>
+  <si>
+    <t>a face</t>
+  </si>
+  <si>
+    <t>a hand</t>
+  </si>
+  <si>
+    <t>a mushroom</t>
+  </si>
+  <si>
+    <t>a piano</t>
+  </si>
+  <si>
+    <t>a spider</t>
+  </si>
+  <si>
+    <t>cdm_run_v7</t>
+  </si>
+  <si>
+    <t>animate</t>
+  </si>
+  <si>
+    <t>a TV</t>
+  </si>
+  <si>
+    <t>an elephant</t>
+  </si>
+  <si>
+    <t>inanimate</t>
   </si>
 </sst>
 </file>
@@ -610,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB08DDAD-1E56-584A-A373-8F3BF63C018F}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:I5"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,22 +624,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -650,13 +650,13 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -667,13 +667,13 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -684,13 +684,13 @@
         <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -701,13 +701,13 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -718,13 +718,13 @@
         <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -735,627 +735,746 @@
         <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
         <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E25" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E31" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E33" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E34" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E35" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E36" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
         <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E37" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
         <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D38" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E38" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B39" t="s">
         <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D39" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E39" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E40" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" t="s">
         <v>39</v>
       </c>
-      <c r="C42" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" t="s">
-        <v>55</v>
-      </c>
-      <c r="E42" t="s">
-        <v>57</v>
+      <c r="C45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" t="s">
+        <v>47</v>
+      </c>
+      <c r="E45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" t="s">
+        <v>47</v>
+      </c>
+      <c r="E47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" t="s">
+        <v>47</v>
+      </c>
+      <c r="E49" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D40" xr:uid="{4C5D514F-3890-6B47-BD1B-495CA6F2C411}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D40">
-      <sortCondition ref="C1:C40"/>
+  <autoFilter ref="A1:D39" xr:uid="{4C5D514F-3890-6B47-BD1B-495CA6F2C411}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D49">
+      <sortCondition ref="D1:D49"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>